<commit_message>
feat: added MAC count
</commit_message>
<xml_diff>
--- a/Final/testing/v2_alexnet/v2_alexnet_results.xlsx
+++ b/Final/testing/v2_alexnet/v2_alexnet_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamkr\Documents\part-4-project\Final\testing\v2_alexnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1479D3D-679E-4148-B3EC-18F44C8E3DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B0E581-15B2-427D-B839-D9BC0A8FDB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>Tile</t>
   </si>
@@ -112,23 +112,22 @@
   </si>
   <si>
     <t>R Latency: modelsim clock cycle output + zero_cols_data_matrix</t>
+  </si>
+  <si>
+    <t>Output Dimension</t>
+  </si>
+  <si>
+    <t>MAC Count (Active PEs)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,17 +147,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -170,23 +164,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -211,12 +208,6 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -231,21 +222,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}" name="Table13" displayName="Table13" ref="A2:H10" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A2:H10" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}" name="Table13" displayName="Table13" ref="A2:I10" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A2:I10" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D227AF0A-A483-4F2B-A0E7-62312D9D0C8A}" name="Tile"/>
     <tableColumn id="2" xr3:uid="{6A12278B-3584-41AA-BE67-5473F1228243}" name="M"/>
     <tableColumn id="3" xr3:uid="{5020DDA2-0D8A-4E35-BEAF-30F287FD75E9}" name="N"/>
     <tableColumn id="4" xr3:uid="{32BEF9DA-5963-4241-AF0C-B51B609CD406}" name="K"/>
-    <tableColumn id="5" xr3:uid="{7E86E347-49CA-41A8-AEFA-54C42A8E7E80}" name="Output Dimension (MAC Count)" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{7E86E347-49CA-41A8-AEFA-54C42A8E7E80}" name="Output Dimension" dataDxfId="8">
       <calculatedColumnFormula>Table13[[#This Row],[M]]*Table13[[#This Row],[K]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D718F0EC-77E4-469F-8D52-F7CA8782BBE8}" name="Latency (Theory)" dataDxfId="6">
+    <tableColumn id="10" xr3:uid="{309554B3-4463-4DED-AFB0-86EDE0A47AE3}" name="MAC Count (Active PEs)"/>
+    <tableColumn id="6" xr3:uid="{D718F0EC-77E4-469F-8D52-F7CA8782BBE8}" name="Latency (Theory)" dataDxfId="7">
       <calculatedColumnFormula>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{92798A34-7BD8-4D26-B8D7-A549814795F6}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{D4FA6A9F-82A1-44DF-9790-64C7064C3DEF}" name="Difference from 3N-2+1" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{D4FA6A9F-82A1-44DF-9790-64C7064C3DEF}" name="Difference from 3N-2+1" dataDxfId="6">
       <calculatedColumnFormula>23-Table13[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -254,21 +246,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}" name="Table134" displayName="Table134" ref="A14:H22" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A14:H22" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}" name="Table134" displayName="Table134" ref="A14:I22" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A14:I22" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DACD87C0-4923-44EE-9D57-1C4490FF2E04}" name="Tile"/>
     <tableColumn id="2" xr3:uid="{C90B1458-DFBB-4BA7-88F9-708DF57453A0}" name="M"/>
     <tableColumn id="3" xr3:uid="{7E1BAA47-9214-4A68-ACDD-84F7D93D5BAD}" name="N"/>
     <tableColumn id="4" xr3:uid="{193B1B2A-056D-41F1-A31A-35DB3CA612E9}" name="K"/>
-    <tableColumn id="5" xr3:uid="{7A3ECADB-1D1A-44FA-90EB-1828A501A260}" name="Output Dimension (MAC Count)" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{7A3ECADB-1D1A-44FA-90EB-1828A501A260}" name="Output Dimension" dataDxfId="4">
       <calculatedColumnFormula>Table134[[#This Row],[M]]*Table134[[#This Row],[K]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F344959C-0D04-4AF5-B2C4-FF7C3F674B16}" name="Latency (Theory)" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{17395CC5-C66A-45BB-AF44-85F63C798FE8}" name="MAC Count (Active PEs)"/>
+    <tableColumn id="6" xr3:uid="{F344959C-0D04-4AF5-B2C4-FF7C3F674B16}" name="Latency (Theory)" dataDxfId="3">
       <calculatedColumnFormula>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{7EEC49AA-4FC8-4A99-9663-A8EEB2AAD5F8}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{B71F4CFD-5FC5-4951-83D9-6674EB7FB889}" name="Difference from 3N-2+1" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{B71F4CFD-5FC5-4951-83D9-6674EB7FB889}" name="Difference from 3N-2+1" dataDxfId="2">
       <calculatedColumnFormula>23-Table134[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -284,14 +277,14 @@
     <tableColumn id="2" xr3:uid="{66D560B9-2DA7-4986-B3DE-CDA502776AC3}" name="M"/>
     <tableColumn id="3" xr3:uid="{5141C682-632F-43C2-8191-BB3609DB4DA8}" name="N"/>
     <tableColumn id="4" xr3:uid="{A9660E6C-180E-485D-A7EB-A8BFCE0C1D97}" name="K"/>
-    <tableColumn id="5" xr3:uid="{34B7FFF0-3EF6-4BA4-A5AB-1660E75007C8}" name="Output Dimension (MAC Count)" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{34B7FFF0-3EF6-4BA4-A5AB-1660E75007C8}" name="Output Dimension (MAC Count)" dataDxfId="1">
       <calculatedColumnFormula>4*8</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{3CE6D932-CF3F-4780-8775-A3AC543F142B}" name="Latency">
       <calculatedColumnFormula>Table1[[#This Row],[M]]+Table1[[#This Row],[N]]+Table1[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{3D0DE0B8-37A2-4603-B02E-4FE79DF8244C}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{78C59BA1-4582-42E9-8A9A-782701EF4A8A}" name="Difference from 3N-2+1" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{78C59BA1-4582-42E9-8A9A-782701EF4A8A}" name="Difference from 3N-2+1" dataDxfId="0">
       <calculatedColumnFormula>23-Table1[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -562,21 +555,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB20B19-942C-4446-8EF3-236D33D3564C}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -584,7 +577,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -598,22 +591,25 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -631,21 +627,24 @@
         <v>32</v>
       </c>
       <c r="F3">
+        <v>32</v>
+      </c>
+      <c r="G3">
         <f>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</f>
         <v>18</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>19</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <f>23-Table13[[#This Row],[Latency (Real)]]</f>
         <v>4</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -663,18 +662,21 @@
         <v>48</v>
       </c>
       <c r="F4">
+        <v>48</v>
+      </c>
+      <c r="G4">
         <f>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</f>
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>21</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <f>23-Table13[[#This Row],[Latency (Real)]]</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -692,18 +694,21 @@
         <v>40</v>
       </c>
       <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="G5">
         <f>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</f>
         <v>19</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>20</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f>23-Table13[[#This Row],[Latency (Real)]]</f>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -721,18 +726,21 @@
         <v>40</v>
       </c>
       <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6">
         <f>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</f>
         <v>19</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>20</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f>23-Table13[[#This Row],[Latency (Real)]]</f>
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -750,18 +758,21 @@
         <v>24</v>
       </c>
       <c r="F7">
+        <v>24</v>
+      </c>
+      <c r="G7">
         <f>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</f>
         <v>17</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>18</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f>23-Table13[[#This Row],[Latency (Real)]]</f>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -779,18 +790,21 @@
         <v>32</v>
       </c>
       <c r="F8">
+        <v>32</v>
+      </c>
+      <c r="G8">
         <f>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</f>
         <v>18</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>19</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f>23-Table13[[#This Row],[Latency (Real)]]</f>
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -808,18 +822,21 @@
         <v>40</v>
       </c>
       <c r="F9">
+        <v>40</v>
+      </c>
+      <c r="G9">
         <f>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</f>
         <v>19</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>20</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f>23-Table13[[#This Row],[Latency (Real)]]</f>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -837,18 +854,21 @@
         <v>16</v>
       </c>
       <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
         <f>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</f>
         <v>16</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>17</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f>23-Table13[[#This Row],[Latency (Real)]]</f>
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -856,7 +876,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -870,48 +890,54 @@
         <v>3</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15" s="3">
-        <v>8</v>
-      </c>
-      <c r="D15" s="3">
-        <v>8</v>
-      </c>
-      <c r="E15" s="3">
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
         <f>Table134[[#This Row],[M]]*Table134[[#This Row],[K]]</f>
         <v>0</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <f>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</f>
         <v>14</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15">
         <v>1</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15">
         <f>23-Table134[[#This Row],[Latency (Real)]]</f>
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -929,18 +955,21 @@
         <v>64</v>
       </c>
       <c r="F16">
+        <v>64</v>
+      </c>
+      <c r="G16">
         <f>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</f>
         <v>22</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>23</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <f>23-Table134[[#This Row],[Latency (Real)]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -958,47 +987,53 @@
         <v>56</v>
       </c>
       <c r="F17">
+        <v>56</v>
+      </c>
+      <c r="G17">
         <f>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</f>
         <v>21</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>22</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f>23-Table134[[#This Row],[Latency (Real)]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18">
         <v>0</v>
       </c>
-      <c r="C18" s="3">
-        <v>8</v>
-      </c>
-      <c r="D18" s="3">
-        <v>8</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
         <f>Table134[[#This Row],[M]]*Table134[[#This Row],[K]]</f>
         <v>0</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
         <f>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</f>
         <v>14</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18">
         <v>1</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18">
         <f>23-Table134[[#This Row],[Latency (Real)]]</f>
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1016,18 +1051,21 @@
         <v>8</v>
       </c>
       <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
         <f>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</f>
         <v>15</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>16</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <f>23-Table134[[#This Row],[Latency (Real)]]</f>
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1045,18 +1083,21 @@
         <v>16</v>
       </c>
       <c r="F20">
+        <v>16</v>
+      </c>
+      <c r="G20">
         <f>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</f>
         <v>16</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>17</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <f>23-Table134[[#This Row],[Latency (Real)]]</f>
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1074,18 +1115,21 @@
         <v>16</v>
       </c>
       <c r="F21">
+        <v>16</v>
+      </c>
+      <c r="G21">
         <f>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</f>
         <v>16</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>17</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <f>23-Table134[[#This Row],[Latency (Real)]]</f>
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1103,19 +1147,22 @@
         <v>24</v>
       </c>
       <c r="F22">
+        <v>24</v>
+      </c>
+      <c r="G22">
         <f>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</f>
         <v>17</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>18</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <f>23-Table134[[#This Row],[Latency (Real)]]</f>
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
@@ -1374,7 +1421,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
feat: got results for nxn baseline
</commit_message>
<xml_diff>
--- a/Final/testing/v2_alexnet/v2_alexnet_results.xlsx
+++ b/Final/testing/v2_alexnet/v2_alexnet_results.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamkr\Documents\part-4-project\Final\testing\v2_alexnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E540CFF-4F15-4D02-8F75-C51DA6917DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFADF8D4-1D54-43CF-927E-D5B1AE4EAE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="old" sheetId="1" r:id="rId2"/>
+    <sheet name="optimised systolic array result" sheetId="3" r:id="rId1"/>
+    <sheet name="baseline systolic array results" sheetId="4" r:id="rId2"/>
+    <sheet name="v2_alexnet" sheetId="2" r:id="rId3"/>
+    <sheet name="old" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
   <si>
     <t>Tile</t>
   </si>
@@ -202,12 +204,90 @@
   </si>
   <si>
     <t xml:space="preserve">demo </t>
+  </si>
+  <si>
+    <t>Row Stripped from Activation Matrix</t>
+  </si>
+  <si>
+    <t>Real Latency (Clock Cycles)</t>
+  </si>
+  <si>
+    <t>Title: Impact on Latency as Row Stripping Increases in a 8x8 Activation</t>
+  </si>
+  <si>
+    <t>Size of Matrix</t>
+  </si>
+  <si>
+    <t>1x8</t>
+  </si>
+  <si>
+    <t>2x8</t>
+  </si>
+  <si>
+    <t>3x8</t>
+  </si>
+  <si>
+    <t>4x8</t>
+  </si>
+  <si>
+    <t>5x8</t>
+  </si>
+  <si>
+    <t>6x8</t>
+  </si>
+  <si>
+    <t>7x8</t>
+  </si>
+  <si>
+    <t>8x8</t>
+  </si>
+  <si>
+    <t>Title: Latency of Baseline Systolic Array on Varying Input Matrix Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tile 0 </t>
+  </si>
+  <si>
+    <t>Tile 8</t>
+  </si>
+  <si>
+    <t>Title: Effect of M value on the number of Active PEs in the Systolic Array and Latency</t>
+  </si>
+  <si>
+    <t>Active PEs (M*N)</t>
+  </si>
+  <si>
+    <t>PE Enabled Mask</t>
+  </si>
+  <si>
+    <t>Title: Latency of Baseline Systolic Array on Different NxN sizes</t>
+  </si>
+  <si>
+    <t>1x1</t>
+  </si>
+  <si>
+    <t>2x2</t>
+  </si>
+  <si>
+    <t>3x3</t>
+  </si>
+  <si>
+    <t>4x4</t>
+  </si>
+  <si>
+    <t>5x5</t>
+  </si>
+  <si>
+    <t>6x6</t>
+  </si>
+  <si>
+    <t>7x7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,17 +331,121 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="27">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9D7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76B1FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE6EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB6C1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -293,7 +477,25 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Pink" pivot="0" count="2" xr9:uid="{6A0DD833-7CB3-4639-B8AC-76E9F8EB74A8}">
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="secondRowStripe" dxfId="15"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{DC0506E3-F402-435F-9F06-5FB0989C3D1B}">
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="secondRowStripe" dxfId="13"/>
+    </tableStyle>
+  </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFB9D7FF"/>
+      <color rgb="FF94C2FF"/>
+      <color rgb="FF76B1FF"/>
+      <color rgb="FFFFE6EE"/>
+      <color rgb="FFFFB6C1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -306,22 +508,76 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}" name="Table13" displayName="Table13" ref="A2:I10" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5981DC08-4755-49EB-B74D-65A5520CC419}" name="Table4" displayName="Table4" ref="A2:B11" totalsRowShown="0">
+  <autoFilter ref="A2:B11" xr:uid="{5981DC08-4755-49EB-B74D-65A5520CC419}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3A7FD3BD-3D73-4E59-8D83-30C3E951A146}" name="Row Stripped from Activation Matrix"/>
+    <tableColumn id="2" xr3:uid="{B9F0620A-F2F2-499C-A905-B0250B4DA68A}" name="Real Latency (Clock Cycles)"/>
+  </tableColumns>
+  <tableStyleInfo name="Pink" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{051A067D-9BFE-4997-9C82-8B3929E18048}" name="Table6" displayName="Table6" ref="D2:J11" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+  <autoFilter ref="D2:J11" xr:uid="{051A067D-9BFE-4997-9C82-8B3929E18048}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{52567FD6-5773-48C8-9C14-6C65CB44DF2D}" name="Tile" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{53E609CF-A8BE-4078-A665-A3835F71A626}" name="M" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{76FB5648-F5C5-491E-802F-ECC5EA1BA0BF}" name="N" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{09E340D5-6267-43EB-9359-76006799FD19}" name="K" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{0708CC41-364D-4680-8AEE-DC69FA135E2C}" name="Active PEs (M*N)" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{22E871CC-1A0D-4470-9916-C2B9F5B93CFD}" name="Latency (Real)" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{4F9CA24C-62DA-4FF4-AC52-BAA10B4B334B}" name="Difference from 3N-2+1" dataDxfId="4">
+      <calculatedColumnFormula>23-I3</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Pink" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{73C64079-F30E-479D-A80B-7BF29F2E9CAF}" name="Table5" displayName="Table5" ref="A2:C10" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="A2:C10" xr:uid="{73C64079-F30E-479D-A80B-7BF29F2E9CAF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{4223D068-5DA5-444E-B53E-3E04385544AC}" name="Size of Matrix" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{94470A14-E7AF-4544-BC5A-343DAEEBAA6A}" name="PE Enabled Mask"/>
+    <tableColumn id="3" xr3:uid="{8E6C3C48-F7B8-428E-B5FD-3855000F9B12}" name="Latency">
+      <calculatedColumnFormula>3*8-2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}" name="Table58" displayName="Table58" ref="G2:H10" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="G2:H10" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{DE127D02-7363-4295-AF36-DDD6DDBD390C}" name="Size of Matrix" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{1F86A7D0-C0ED-4BD0-8855-C8E934AD579D}" name="Latency"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}" name="Table13" displayName="Table13" ref="A2:I10" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A2:I10" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D227AF0A-A483-4F2B-A0E7-62312D9D0C8A}" name="Tile"/>
     <tableColumn id="2" xr3:uid="{6A12278B-3584-41AA-BE67-5473F1228243}" name="M"/>
     <tableColumn id="3" xr3:uid="{5020DDA2-0D8A-4E35-BEAF-30F287FD75E9}" name="N"/>
     <tableColumn id="4" xr3:uid="{32BEF9DA-5963-4241-AF0C-B51B609CD406}" name="K"/>
-    <tableColumn id="5" xr3:uid="{7E86E347-49CA-41A8-AEFA-54C42A8E7E80}" name="Output Dimension" dataDxfId="8">
+    <tableColumn id="5" xr3:uid="{7E86E347-49CA-41A8-AEFA-54C42A8E7E80}" name="Output Dimension" dataDxfId="25">
       <calculatedColumnFormula>Table13[[#This Row],[M]]*Table13[[#This Row],[K]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{309554B3-4463-4DED-AFB0-86EDE0A47AE3}" name="MAC Count (Active PEs)"/>
-    <tableColumn id="6" xr3:uid="{D718F0EC-77E4-469F-8D52-F7CA8782BBE8}" name="Latency (Theory)" dataDxfId="7">
+    <tableColumn id="6" xr3:uid="{D718F0EC-77E4-469F-8D52-F7CA8782BBE8}" name="Latency (Theory)" dataDxfId="24">
       <calculatedColumnFormula>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{92798A34-7BD8-4D26-B8D7-A549814795F6}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{D4FA6A9F-82A1-44DF-9790-64C7064C3DEF}" name="Difference from 3N-2+1" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{D4FA6A9F-82A1-44DF-9790-64C7064C3DEF}" name="Difference from 3N-2+1" dataDxfId="23">
       <calculatedColumnFormula>23-Table13[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -329,23 +585,23 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}" name="Table134" displayName="Table134" ref="A14:I22" totalsRowShown="0" headerRowDxfId="5">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}" name="Table134" displayName="Table134" ref="A14:I22" totalsRowShown="0" headerRowDxfId="22">
   <autoFilter ref="A14:I22" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DACD87C0-4923-44EE-9D57-1C4490FF2E04}" name="Tile"/>
     <tableColumn id="2" xr3:uid="{C90B1458-DFBB-4BA7-88F9-708DF57453A0}" name="M"/>
     <tableColumn id="3" xr3:uid="{7E1BAA47-9214-4A68-ACDD-84F7D93D5BAD}" name="N"/>
     <tableColumn id="4" xr3:uid="{193B1B2A-056D-41F1-A31A-35DB3CA612E9}" name="K"/>
-    <tableColumn id="5" xr3:uid="{7A3ECADB-1D1A-44FA-90EB-1828A501A260}" name="Output Dimension" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{7A3ECADB-1D1A-44FA-90EB-1828A501A260}" name="Output Dimension" dataDxfId="21">
       <calculatedColumnFormula>Table134[[#This Row],[M]]*Table134[[#This Row],[K]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{17395CC5-C66A-45BB-AF44-85F63C798FE8}" name="MAC Count (Active PEs)"/>
-    <tableColumn id="6" xr3:uid="{F344959C-0D04-4AF5-B2C4-FF7C3F674B16}" name="Latency (Theory)" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{F344959C-0D04-4AF5-B2C4-FF7C3F674B16}" name="Latency (Theory)" dataDxfId="20">
       <calculatedColumnFormula>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{7EEC49AA-4FC8-4A99-9663-A8EEB2AAD5F8}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{B71F4CFD-5FC5-4951-83D9-6674EB7FB889}" name="Difference from 3N-2+1" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{B71F4CFD-5FC5-4951-83D9-6674EB7FB889}" name="Difference from 3N-2+1" dataDxfId="19">
       <calculatedColumnFormula>23-Table134[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -353,7 +609,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA1FDD35-9C8D-43D3-A42C-5D9448260A9A}" name="Table1" displayName="Table1" ref="A2:H10" totalsRowShown="0">
   <autoFilter ref="A2:H10" xr:uid="{BA1FDD35-9C8D-43D3-A42C-5D9448260A9A}"/>
   <tableColumns count="8">
@@ -361,14 +617,14 @@
     <tableColumn id="2" xr3:uid="{66D560B9-2DA7-4986-B3DE-CDA502776AC3}" name="M"/>
     <tableColumn id="3" xr3:uid="{5141C682-632F-43C2-8191-BB3609DB4DA8}" name="N"/>
     <tableColumn id="4" xr3:uid="{A9660E6C-180E-485D-A7EB-A8BFCE0C1D97}" name="K"/>
-    <tableColumn id="5" xr3:uid="{34B7FFF0-3EF6-4BA4-A5AB-1660E75007C8}" name="Output Dimension (MAC Count)" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{34B7FFF0-3EF6-4BA4-A5AB-1660E75007C8}" name="Output Dimension (MAC Count)" dataDxfId="18">
       <calculatedColumnFormula>4*8</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{3CE6D932-CF3F-4780-8775-A3AC543F142B}" name="Latency">
       <calculatedColumnFormula>Table1[[#This Row],[M]]+Table1[[#This Row],[N]]+Table1[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{3D0DE0B8-37A2-4603-B02E-4FE79DF8244C}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{78C59BA1-4582-42E9-8A9A-782701EF4A8A}" name="Difference from 3N-2+1" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{78C59BA1-4582-42E9-8A9A-782701EF4A8A}" name="Difference from 3N-2+1" dataDxfId="17">
       <calculatedColumnFormula>23-Table1[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -638,11 +894,545 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EAF263-E46A-4974-93A7-B91CE9F0B8F1}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3">
+        <v>8</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5">
+        <f>23-I3</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>22</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5">
+        <v>16</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" ref="J4:J11" si="0">23-I4</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5">
+        <v>16</v>
+      </c>
+      <c r="I5" s="5">
+        <v>17</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5">
+        <v>24</v>
+      </c>
+      <c r="I6" s="5">
+        <v>18</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3">
+        <v>8</v>
+      </c>
+      <c r="H7" s="5">
+        <v>32</v>
+      </c>
+      <c r="I7" s="5">
+        <v>19</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3">
+        <v>8</v>
+      </c>
+      <c r="H8" s="5">
+        <v>40</v>
+      </c>
+      <c r="I8" s="5">
+        <v>20</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3">
+        <v>8</v>
+      </c>
+      <c r="H9" s="5">
+        <v>48</v>
+      </c>
+      <c r="I9" s="5">
+        <v>21</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3">
+        <v>8</v>
+      </c>
+      <c r="H10" s="5">
+        <v>56</v>
+      </c>
+      <c r="I10" s="5">
+        <v>22</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3">
+        <v>8</v>
+      </c>
+      <c r="H11" s="5">
+        <v>64</v>
+      </c>
+      <c r="I11" s="5">
+        <v>23</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:J1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4BB971-1A81-4E50-9B97-4F8E57E392C9}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="212" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3">
+        <f>3*8-2</f>
+        <v>22</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C10" si="0">3*8-2</f>
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB20B19-942C-4446-8EF3-236D33D3564C}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView zoomScale="134" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +1441,7 @@
     <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1360,7 +2150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>

</xml_diff>

<commit_message>
feat: added nxn as newcommands
</commit_message>
<xml_diff>
--- a/Final/testing/v2_alexnet/v2_alexnet_results.xlsx
+++ b/Final/testing/v2_alexnet/v2_alexnet_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamkr\Documents\part-4-project\Final\testing\v2_alexnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFADF8D4-1D54-43CF-927E-D5B1AE4EAE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1E6940-E2CE-4589-8D96-EEDBF1545204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -331,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -341,31 +341,91 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b/>
       </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -387,38 +447,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFB9D7FF"/>
@@ -446,45 +474,15 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Pink" pivot="0" count="2" xr9:uid="{6A0DD833-7CB3-4639-B8AC-76E9F8EB74A8}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="secondRowStripe" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="secondRowStripe" dxfId="25"/>
     </tableStyle>
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{DC0506E3-F402-435F-9F06-5FB0989C3D1B}">
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="secondRowStripe" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="24"/>
+      <tableStyleElement type="secondRowStripe" dxfId="23"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -519,16 +517,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{051A067D-9BFE-4997-9C82-8B3929E18048}" name="Table6" displayName="Table6" ref="D2:J11" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{051A067D-9BFE-4997-9C82-8B3929E18048}" name="Table6" displayName="Table6" ref="D2:J11" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="D2:J11" xr:uid="{051A067D-9BFE-4997-9C82-8B3929E18048}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{52567FD6-5773-48C8-9C14-6C65CB44DF2D}" name="Tile" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{53E609CF-A8BE-4078-A665-A3835F71A626}" name="M" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{76FB5648-F5C5-491E-802F-ECC5EA1BA0BF}" name="N" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{09E340D5-6267-43EB-9359-76006799FD19}" name="K" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{0708CC41-364D-4680-8AEE-DC69FA135E2C}" name="Active PEs (M*N)" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{22E871CC-1A0D-4470-9916-C2B9F5B93CFD}" name="Latency (Real)" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{4F9CA24C-62DA-4FF4-AC52-BAA10B4B334B}" name="Difference from 3N-2+1" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{52567FD6-5773-48C8-9C14-6C65CB44DF2D}" name="Tile" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{53E609CF-A8BE-4078-A665-A3835F71A626}" name="M" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{76FB5648-F5C5-491E-802F-ECC5EA1BA0BF}" name="N" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{09E340D5-6267-43EB-9359-76006799FD19}" name="K" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{0708CC41-364D-4680-8AEE-DC69FA135E2C}" name="Active PEs (M*N)" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{22E871CC-1A0D-4470-9916-C2B9F5B93CFD}" name="Latency (Real)" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{4F9CA24C-62DA-4FF4-AC52-BAA10B4B334B}" name="Difference from 3N-2+1" dataDxfId="14">
       <calculatedColumnFormula>23-I3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -537,10 +535,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{73C64079-F30E-479D-A80B-7BF29F2E9CAF}" name="Table5" displayName="Table5" ref="A2:C10" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{73C64079-F30E-479D-A80B-7BF29F2E9CAF}" name="Table5" displayName="Table5" ref="A2:C10" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A2:C10" xr:uid="{73C64079-F30E-479D-A80B-7BF29F2E9CAF}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4223D068-5DA5-444E-B53E-3E04385544AC}" name="Size of Matrix" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{4223D068-5DA5-444E-B53E-3E04385544AC}" name="Size of Matrix" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{94470A14-E7AF-4544-BC5A-343DAEEBAA6A}" name="PE Enabled Mask"/>
     <tableColumn id="3" xr3:uid="{8E6C3C48-F7B8-428E-B5FD-3855000F9B12}" name="Latency">
       <calculatedColumnFormula>3*8-2</calculatedColumnFormula>
@@ -551,10 +549,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}" name="Table58" displayName="Table58" ref="G2:H10" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}" name="Table58" displayName="Table58" ref="G2:H10" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="G2:H10" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DE127D02-7363-4295-AF36-DDD6DDBD390C}" name="Size of Matrix" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{DE127D02-7363-4295-AF36-DDD6DDBD390C}" name="Size of Matrix" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{1F86A7D0-C0ED-4BD0-8855-C8E934AD579D}" name="Latency"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -562,22 +560,22 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}" name="Table13" displayName="Table13" ref="A2:I10" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}" name="Table13" displayName="Table13" ref="A2:I10" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A2:I10" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D227AF0A-A483-4F2B-A0E7-62312D9D0C8A}" name="Tile"/>
     <tableColumn id="2" xr3:uid="{6A12278B-3584-41AA-BE67-5473F1228243}" name="M"/>
     <tableColumn id="3" xr3:uid="{5020DDA2-0D8A-4E35-BEAF-30F287FD75E9}" name="N"/>
     <tableColumn id="4" xr3:uid="{32BEF9DA-5963-4241-AF0C-B51B609CD406}" name="K"/>
-    <tableColumn id="5" xr3:uid="{7E86E347-49CA-41A8-AEFA-54C42A8E7E80}" name="Output Dimension" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{7E86E347-49CA-41A8-AEFA-54C42A8E7E80}" name="Output Dimension" dataDxfId="8">
       <calculatedColumnFormula>Table13[[#This Row],[M]]*Table13[[#This Row],[K]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{309554B3-4463-4DED-AFB0-86EDE0A47AE3}" name="MAC Count (Active PEs)"/>
-    <tableColumn id="6" xr3:uid="{D718F0EC-77E4-469F-8D52-F7CA8782BBE8}" name="Latency (Theory)" dataDxfId="24">
+    <tableColumn id="6" xr3:uid="{D718F0EC-77E4-469F-8D52-F7CA8782BBE8}" name="Latency (Theory)" dataDxfId="7">
       <calculatedColumnFormula>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{92798A34-7BD8-4D26-B8D7-A549814795F6}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{D4FA6A9F-82A1-44DF-9790-64C7064C3DEF}" name="Difference from 3N-2+1" dataDxfId="23">
+    <tableColumn id="8" xr3:uid="{D4FA6A9F-82A1-44DF-9790-64C7064C3DEF}" name="Difference from 3N-2+1" dataDxfId="6">
       <calculatedColumnFormula>23-Table13[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -586,22 +584,22 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}" name="Table134" displayName="Table134" ref="A14:I22" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}" name="Table134" displayName="Table134" ref="A14:I22" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A14:I22" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DACD87C0-4923-44EE-9D57-1C4490FF2E04}" name="Tile"/>
     <tableColumn id="2" xr3:uid="{C90B1458-DFBB-4BA7-88F9-708DF57453A0}" name="M"/>
     <tableColumn id="3" xr3:uid="{7E1BAA47-9214-4A68-ACDD-84F7D93D5BAD}" name="N"/>
     <tableColumn id="4" xr3:uid="{193B1B2A-056D-41F1-A31A-35DB3CA612E9}" name="K"/>
-    <tableColumn id="5" xr3:uid="{7A3ECADB-1D1A-44FA-90EB-1828A501A260}" name="Output Dimension" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{7A3ECADB-1D1A-44FA-90EB-1828A501A260}" name="Output Dimension" dataDxfId="4">
       <calculatedColumnFormula>Table134[[#This Row],[M]]*Table134[[#This Row],[K]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{17395CC5-C66A-45BB-AF44-85F63C798FE8}" name="MAC Count (Active PEs)"/>
-    <tableColumn id="6" xr3:uid="{F344959C-0D04-4AF5-B2C4-FF7C3F674B16}" name="Latency (Theory)" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{F344959C-0D04-4AF5-B2C4-FF7C3F674B16}" name="Latency (Theory)" dataDxfId="3">
       <calculatedColumnFormula>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{7EEC49AA-4FC8-4A99-9663-A8EEB2AAD5F8}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{B71F4CFD-5FC5-4951-83D9-6674EB7FB889}" name="Difference from 3N-2+1" dataDxfId="19">
+    <tableColumn id="8" xr3:uid="{B71F4CFD-5FC5-4951-83D9-6674EB7FB889}" name="Difference from 3N-2+1" dataDxfId="2">
       <calculatedColumnFormula>23-Table134[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -617,14 +615,14 @@
     <tableColumn id="2" xr3:uid="{66D560B9-2DA7-4986-B3DE-CDA502776AC3}" name="M"/>
     <tableColumn id="3" xr3:uid="{5141C682-632F-43C2-8191-BB3609DB4DA8}" name="N"/>
     <tableColumn id="4" xr3:uid="{A9660E6C-180E-485D-A7EB-A8BFCE0C1D97}" name="K"/>
-    <tableColumn id="5" xr3:uid="{34B7FFF0-3EF6-4BA4-A5AB-1660E75007C8}" name="Output Dimension (MAC Count)" dataDxfId="18">
+    <tableColumn id="5" xr3:uid="{34B7FFF0-3EF6-4BA4-A5AB-1660E75007C8}" name="Output Dimension (MAC Count)" dataDxfId="1">
       <calculatedColumnFormula>4*8</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{3CE6D932-CF3F-4780-8775-A3AC543F142B}" name="Latency">
       <calculatedColumnFormula>Table1[[#This Row],[M]]+Table1[[#This Row],[N]]+Table1[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{3D0DE0B8-37A2-4603-B02E-4FE79DF8244C}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{78C59BA1-4582-42E9-8A9A-782701EF4A8A}" name="Difference from 3N-2+1" dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{78C59BA1-4582-42E9-8A9A-782701EF4A8A}" name="Difference from 3N-2+1" dataDxfId="0">
       <calculatedColumnFormula>23-Table1[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -898,7 +896,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:J11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,57 +913,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3">
         <v>0</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3">
         <v>23</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E3" s="3">
@@ -977,25 +975,25 @@
       <c r="G3" s="3">
         <v>8</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>1</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <f>23-I3</f>
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4">
         <v>22</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="3">
@@ -1007,25 +1005,25 @@
       <c r="G4" s="3">
         <v>8</v>
       </c>
-      <c r="H4" s="5">
-        <v>8</v>
-      </c>
-      <c r="I4" s="5">
+      <c r="H4" s="4">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4">
         <v>16</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <f t="shared" ref="J4:J11" si="0">23-I4</f>
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5">
         <v>21</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="3">
@@ -1037,25 +1035,25 @@
       <c r="G5" s="3">
         <v>8</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>16</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>17</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6">
         <v>20</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="3">
@@ -1067,25 +1065,25 @@
       <c r="G6" s="3">
         <v>8</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>24</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>18</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7">
         <v>19</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="3">
@@ -1097,25 +1095,25 @@
       <c r="G7" s="3">
         <v>8</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>32</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>19</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8">
         <v>18</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="3">
@@ -1127,25 +1125,25 @@
       <c r="G8" s="3">
         <v>8</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>40</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>20</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9">
         <v>17</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="3">
@@ -1157,25 +1155,25 @@
       <c r="G9" s="3">
         <v>8</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>48</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>21</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10">
         <v>16</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="3">
@@ -1187,25 +1185,25 @@
       <c r="G10" s="3">
         <v>8</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>56</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>22</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>8</v>
-      </c>
-      <c r="B11" s="7">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E11" s="3">
@@ -1217,13 +1215,13 @@
       <c r="G11" s="3">
         <v>8</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>64</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>23</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1246,7 +1244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4BB971-1A81-4E50-9B97-4F8E57E392C9}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="212" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="230" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -1259,22 +1257,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1294,14 +1292,14 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C3">
         <f>3*8-2</f>
         <v>22</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>74</v>
       </c>
       <c r="H3">
@@ -1309,14 +1307,14 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C10" si="0">3*8-2</f>
         <v>22</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="5" t="s">
         <v>75</v>
       </c>
       <c r="H4">
@@ -1324,14 +1322,14 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>76</v>
       </c>
       <c r="H5">
@@ -1339,14 +1337,14 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="5" t="s">
         <v>77</v>
       </c>
       <c r="H6">
@@ -1354,14 +1352,14 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="5" t="s">
         <v>78</v>
       </c>
       <c r="H7">
@@ -1369,14 +1367,14 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>79</v>
       </c>
       <c r="H8">
@@ -1384,14 +1382,14 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="5" t="s">
         <v>80</v>
       </c>
       <c r="H9">
@@ -1399,14 +1397,14 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="5" t="s">
         <v>66</v>
       </c>
       <c r="H10">

</xml_diff>

<commit_message>
feat: collated screenshots of varying m sizes for optimsied
</commit_message>
<xml_diff>
--- a/Final/testing/v2_alexnet/v2_alexnet_results.xlsx
+++ b/Final/testing/v2_alexnet/v2_alexnet_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamkr\Documents\part-4-project\Final\testing\v2_alexnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE4D93-2FA9-4474-97E8-85895B6290FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F80DCC0-1582-4822-A552-888107B5C85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="optimised systolic array result" sheetId="3" r:id="rId1"/>
@@ -334,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -355,19 +355,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -404,6 +397,12 @@
       <font>
         <b/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -549,8 +548,8 @@
   <autoFilter ref="A2:C10" xr:uid="{73C64079-F30E-479D-A80B-7BF29F2E9CAF}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{4223D068-5DA5-444E-B53E-3E04385544AC}" name="Size of Matrix A" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{D6124365-E85B-4316-9744-B5FA106748A8}" name="Size of Matrix B" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{8E6C3C48-F7B8-428E-B5FD-3855000F9B12}" name="Latency" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{D6124365-E85B-4316-9744-B5FA106748A8}" name="Size of Matrix B" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{8E6C3C48-F7B8-428E-B5FD-3855000F9B12}" name="Latency" dataDxfId="12">
       <calculatedColumnFormula>3*8-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -559,10 +558,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}" name="Table58" displayName="Table58" ref="G2:H10" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}" name="Table58" displayName="Table58" ref="G2:H10" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="G2:H10" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DE127D02-7363-4295-AF36-DDD6DDBD390C}" name="Size of Matrix A and Matrix B" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{DE127D02-7363-4295-AF36-DDD6DDBD390C}" name="Size of Matrix A and Matrix B" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{1F86A7D0-C0ED-4BD0-8855-C8E934AD579D}" name="Latency"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -570,22 +569,22 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}" name="Table13" displayName="Table13" ref="A2:I10" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}" name="Table13" displayName="Table13" ref="A2:I10" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A2:I10" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D227AF0A-A483-4F2B-A0E7-62312D9D0C8A}" name="Tile"/>
     <tableColumn id="2" xr3:uid="{6A12278B-3584-41AA-BE67-5473F1228243}" name="M"/>
     <tableColumn id="3" xr3:uid="{5020DDA2-0D8A-4E35-BEAF-30F287FD75E9}" name="N"/>
     <tableColumn id="4" xr3:uid="{32BEF9DA-5963-4241-AF0C-B51B609CD406}" name="K"/>
-    <tableColumn id="5" xr3:uid="{7E86E347-49CA-41A8-AEFA-54C42A8E7E80}" name="Output Dimension" dataDxfId="10">
+    <tableColumn id="5" xr3:uid="{7E86E347-49CA-41A8-AEFA-54C42A8E7E80}" name="Output Dimension" dataDxfId="8">
       <calculatedColumnFormula>Table13[[#This Row],[M]]*Table13[[#This Row],[K]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{309554B3-4463-4DED-AFB0-86EDE0A47AE3}" name="MAC Count (Active PEs)"/>
-    <tableColumn id="6" xr3:uid="{D718F0EC-77E4-469F-8D52-F7CA8782BBE8}" name="Latency (Theory)" dataDxfId="9">
+    <tableColumn id="6" xr3:uid="{D718F0EC-77E4-469F-8D52-F7CA8782BBE8}" name="Latency (Theory)" dataDxfId="7">
       <calculatedColumnFormula>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{92798A34-7BD8-4D26-B8D7-A549814795F6}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{D4FA6A9F-82A1-44DF-9790-64C7064C3DEF}" name="Difference from 3N-2+1" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{D4FA6A9F-82A1-44DF-9790-64C7064C3DEF}" name="Difference from 3N-2+1" dataDxfId="6">
       <calculatedColumnFormula>23-Table13[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -594,22 +593,22 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}" name="Table134" displayName="Table134" ref="A14:I22" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}" name="Table134" displayName="Table134" ref="A14:I22" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A14:I22" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DACD87C0-4923-44EE-9D57-1C4490FF2E04}" name="Tile"/>
     <tableColumn id="2" xr3:uid="{C90B1458-DFBB-4BA7-88F9-708DF57453A0}" name="M"/>
     <tableColumn id="3" xr3:uid="{7E1BAA47-9214-4A68-ACDD-84F7D93D5BAD}" name="N"/>
     <tableColumn id="4" xr3:uid="{193B1B2A-056D-41F1-A31A-35DB3CA612E9}" name="K"/>
-    <tableColumn id="5" xr3:uid="{7A3ECADB-1D1A-44FA-90EB-1828A501A260}" name="Output Dimension" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{7A3ECADB-1D1A-44FA-90EB-1828A501A260}" name="Output Dimension" dataDxfId="4">
       <calculatedColumnFormula>Table134[[#This Row],[M]]*Table134[[#This Row],[K]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{17395CC5-C66A-45BB-AF44-85F63C798FE8}" name="MAC Count (Active PEs)"/>
-    <tableColumn id="6" xr3:uid="{F344959C-0D04-4AF5-B2C4-FF7C3F674B16}" name="Latency (Theory)" dataDxfId="5">
+    <tableColumn id="6" xr3:uid="{F344959C-0D04-4AF5-B2C4-FF7C3F674B16}" name="Latency (Theory)" dataDxfId="3">
       <calculatedColumnFormula>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{7EEC49AA-4FC8-4A99-9663-A8EEB2AAD5F8}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{B71F4CFD-5FC5-4951-83D9-6674EB7FB889}" name="Difference from 3N-2+1" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{B71F4CFD-5FC5-4951-83D9-6674EB7FB889}" name="Difference from 3N-2+1" dataDxfId="2">
       <calculatedColumnFormula>23-Table134[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -625,14 +624,14 @@
     <tableColumn id="2" xr3:uid="{66D560B9-2DA7-4986-B3DE-CDA502776AC3}" name="M"/>
     <tableColumn id="3" xr3:uid="{5141C682-632F-43C2-8191-BB3609DB4DA8}" name="N"/>
     <tableColumn id="4" xr3:uid="{A9660E6C-180E-485D-A7EB-A8BFCE0C1D97}" name="K"/>
-    <tableColumn id="5" xr3:uid="{34B7FFF0-3EF6-4BA4-A5AB-1660E75007C8}" name="Output Dimension (MAC Count)" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{34B7FFF0-3EF6-4BA4-A5AB-1660E75007C8}" name="Output Dimension (MAC Count)" dataDxfId="1">
       <calculatedColumnFormula>4*8</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{3CE6D932-CF3F-4780-8775-A3AC543F142B}" name="Latency">
       <calculatedColumnFormula>Table1[[#This Row],[M]]+Table1[[#This Row],[N]]+Table1[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{3D0DE0B8-37A2-4603-B02E-4FE79DF8244C}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{78C59BA1-4582-42E9-8A9A-782701EF4A8A}" name="Difference from 3N-2+1" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{78C59BA1-4582-42E9-8A9A-782701EF4A8A}" name="Difference from 3N-2+1" dataDxfId="0">
       <calculatedColumnFormula>23-Table1[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -906,7 +905,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4BB971-1A81-4E50-9B97-4F8E57E392C9}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="181" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1273,9 +1272,6 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
       <c r="G1" s="7" t="s">
         <v>71</v>
       </c>
@@ -1464,13 +1460,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB20B19-942C-4446-8EF3-236D33D3564C}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="134" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
feat: performance analysis done but has compilation error
</commit_message>
<xml_diff>
--- a/Final/testing/v2_alexnet/v2_alexnet_results.xlsx
+++ b/Final/testing/v2_alexnet/v2_alexnet_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamkr\Documents\part-4-project\Final\testing\v2_alexnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F80DCC0-1582-4822-A552-888107B5C85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6396DDC5-DC67-471A-B2B0-6E16B5998FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="optimised systolic array result" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="86">
   <si>
     <t>Tile</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Real Latency (Clock Cycles)</t>
   </si>
   <si>
-    <t>Title: Impact on Latency as Row Stripping Increases in a 8x8 Activation</t>
-  </si>
-  <si>
     <t>1x8</t>
   </si>
   <si>
@@ -285,6 +282,21 @@
   </si>
   <si>
     <t>Size of Matrix A and Matrix B</t>
+  </si>
+  <si>
+    <t>Sparsity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock Cycles - Model Sim </t>
+  </si>
+  <si>
+    <t>Title: Impact of Stripping Algorithm on Clock Cycles when Applied on Random Sparsity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title: </t>
+  </si>
+  <si>
+    <t>Difference from Baseline</t>
   </si>
 </sst>
 </file>
@@ -359,7 +371,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -486,21 +503,21 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Pink" pivot="0" count="2" xr9:uid="{6A0DD833-7CB3-4639-B8AC-76E9F8EB74A8}">
-      <tableStyleElement type="headerRow" dxfId="28"/>
-      <tableStyleElement type="secondRowStripe" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="29"/>
+      <tableStyleElement type="secondRowStripe" dxfId="28"/>
     </tableStyle>
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{DC0506E3-F402-435F-9F06-5FB0989C3D1B}">
-      <tableStyleElement type="headerRow" dxfId="26"/>
-      <tableStyleElement type="secondRowStripe" dxfId="25"/>
+      <tableStyleElement type="headerRow" dxfId="27"/>
+      <tableStyleElement type="secondRowStripe" dxfId="26"/>
     </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFFE6EE"/>
+      <color rgb="FFFFB6C1"/>
+      <color rgb="FF76B1FF"/>
       <color rgb="FFB9D7FF"/>
       <color rgb="FF94C2FF"/>
-      <color rgb="FF76B1FF"/>
-      <color rgb="FFFFE6EE"/>
-      <color rgb="FFFFB6C1"/>
     </mruColors>
   </colors>
   <extLst>
@@ -512,6 +529,1064 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>Impact on Latency as Row Stripping Increases in a 8x8 Activation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'optimised systolic array result'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real Latency (Clock Cycles)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'optimised systolic array result'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'optimised systolic array result'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ACCA-49DB-81A1-0840F040D458}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1067495456"/>
+        <c:axId val="1067493536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1067495456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Real</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> Latency (Clock Cycles</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1067493536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1067493536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Row</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> Stripped From Activation Matrix</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1067495456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2109496</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28757</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431020</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>61591</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{158A6608-3279-4F1F-C99C-D7706B18F013}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,16 +1601,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{051A067D-9BFE-4997-9C82-8B3929E18048}" name="Table6" displayName="Table6" ref="D2:J11" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{051A067D-9BFE-4997-9C82-8B3929E18048}" name="Table6" displayName="Table6" ref="D2:J11" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="D2:J11" xr:uid="{051A067D-9BFE-4997-9C82-8B3929E18048}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{52567FD6-5773-48C8-9C14-6C65CB44DF2D}" name="Tile" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{53E609CF-A8BE-4078-A665-A3835F71A626}" name="M" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{76FB5648-F5C5-491E-802F-ECC5EA1BA0BF}" name="N" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{09E340D5-6267-43EB-9359-76006799FD19}" name="K" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{0708CC41-364D-4680-8AEE-DC69FA135E2C}" name="Active PEs (M*N)" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{22E871CC-1A0D-4470-9916-C2B9F5B93CFD}" name="Latency (Real)" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{4F9CA24C-62DA-4FF4-AC52-BAA10B4B334B}" name="Difference from 3N-2+1" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{52567FD6-5773-48C8-9C14-6C65CB44DF2D}" name="Tile" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{53E609CF-A8BE-4078-A665-A3835F71A626}" name="M" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{76FB5648-F5C5-491E-802F-ECC5EA1BA0BF}" name="N" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{09E340D5-6267-43EB-9359-76006799FD19}" name="K" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{0708CC41-364D-4680-8AEE-DC69FA135E2C}" name="Active PEs (M*N)" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{22E871CC-1A0D-4470-9916-C2B9F5B93CFD}" name="Latency (Real)" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{4F9CA24C-62DA-4FF4-AC52-BAA10B4B334B}" name="Difference from Baseline" dataDxfId="17">
       <calculatedColumnFormula>23-I3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -544,12 +1619,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{73C64079-F30E-479D-A80B-7BF29F2E9CAF}" name="Table5" displayName="Table5" ref="A2:C10" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FE9EBA62-87A6-48DE-9FD0-115C9888FB6D}" name="Table8" displayName="Table8" ref="L2:M15" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="L2:M15" xr:uid="{FE9EBA62-87A6-48DE-9FD0-115C9888FB6D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{153C72B5-F301-4381-83B2-9C6CB91D79D0}" name="Sparsity"/>
+    <tableColumn id="2" xr3:uid="{4BC7112A-433C-447B-A157-12834E7A89E6}" name="Clock Cycles - Model Sim "/>
+  </tableColumns>
+  <tableStyleInfo name="Pink" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{73C64079-F30E-479D-A80B-7BF29F2E9CAF}" name="Table5" displayName="Table5" ref="A2:C10" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A2:C10" xr:uid="{73C64079-F30E-479D-A80B-7BF29F2E9CAF}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4223D068-5DA5-444E-B53E-3E04385544AC}" name="Size of Matrix A" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{D6124365-E85B-4316-9744-B5FA106748A8}" name="Size of Matrix B" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{8E6C3C48-F7B8-428E-B5FD-3855000F9B12}" name="Latency" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{4223D068-5DA5-444E-B53E-3E04385544AC}" name="Size of Matrix A" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D6124365-E85B-4316-9744-B5FA106748A8}" name="Size of Matrix B" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{8E6C3C48-F7B8-428E-B5FD-3855000F9B12}" name="Latency" dataDxfId="13">
       <calculatedColumnFormula>3*8-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -557,34 +1643,34 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}" name="Table58" displayName="Table58" ref="G2:H10" totalsRowShown="0" headerRowDxfId="11">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}" name="Table58" displayName="Table58" ref="G2:H10" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="G2:H10" xr:uid="{3838693E-2926-4C79-A48B-2D9D94DA33FB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DE127D02-7363-4295-AF36-DDD6DDBD390C}" name="Size of Matrix A and Matrix B" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{DE127D02-7363-4295-AF36-DDD6DDBD390C}" name="Size of Matrix A and Matrix B" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{1F86A7D0-C0ED-4BD0-8855-C8E934AD579D}" name="Latency"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}" name="Table13" displayName="Table13" ref="A2:I10" totalsRowShown="0" headerRowDxfId="9">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}" name="Table13" displayName="Table13" ref="A2:I10" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A2:I10" xr:uid="{B8E41667-AB07-4658-B8AC-6CD371733CB2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D227AF0A-A483-4F2B-A0E7-62312D9D0C8A}" name="Tile"/>
     <tableColumn id="2" xr3:uid="{6A12278B-3584-41AA-BE67-5473F1228243}" name="M"/>
     <tableColumn id="3" xr3:uid="{5020DDA2-0D8A-4E35-BEAF-30F287FD75E9}" name="N"/>
     <tableColumn id="4" xr3:uid="{32BEF9DA-5963-4241-AF0C-B51B609CD406}" name="K"/>
-    <tableColumn id="5" xr3:uid="{7E86E347-49CA-41A8-AEFA-54C42A8E7E80}" name="Output Dimension" dataDxfId="8">
+    <tableColumn id="5" xr3:uid="{7E86E347-49CA-41A8-AEFA-54C42A8E7E80}" name="Output Dimension" dataDxfId="9">
       <calculatedColumnFormula>Table13[[#This Row],[M]]*Table13[[#This Row],[K]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{309554B3-4463-4DED-AFB0-86EDE0A47AE3}" name="MAC Count (Active PEs)"/>
-    <tableColumn id="6" xr3:uid="{D718F0EC-77E4-469F-8D52-F7CA8782BBE8}" name="Latency (Theory)" dataDxfId="7">
+    <tableColumn id="6" xr3:uid="{D718F0EC-77E4-469F-8D52-F7CA8782BBE8}" name="Latency (Theory)" dataDxfId="8">
       <calculatedColumnFormula>Table13[[#This Row],[M]]+Table13[[#This Row],[N]]+Table13[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{92798A34-7BD8-4D26-B8D7-A549814795F6}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{D4FA6A9F-82A1-44DF-9790-64C7064C3DEF}" name="Difference from 3N-2+1" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{D4FA6A9F-82A1-44DF-9790-64C7064C3DEF}" name="Difference from 3N-2+1" dataDxfId="7">
       <calculatedColumnFormula>23-Table13[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -592,23 +1678,23 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}" name="Table134" displayName="Table134" ref="A14:I22" totalsRowShown="0" headerRowDxfId="5">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}" name="Table134" displayName="Table134" ref="A14:I22" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A14:I22" xr:uid="{B811506F-69AF-479D-81D3-30BB15DDDBFD}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DACD87C0-4923-44EE-9D57-1C4490FF2E04}" name="Tile"/>
     <tableColumn id="2" xr3:uid="{C90B1458-DFBB-4BA7-88F9-708DF57453A0}" name="M"/>
     <tableColumn id="3" xr3:uid="{7E1BAA47-9214-4A68-ACDD-84F7D93D5BAD}" name="N"/>
     <tableColumn id="4" xr3:uid="{193B1B2A-056D-41F1-A31A-35DB3CA612E9}" name="K"/>
-    <tableColumn id="5" xr3:uid="{7A3ECADB-1D1A-44FA-90EB-1828A501A260}" name="Output Dimension" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{7A3ECADB-1D1A-44FA-90EB-1828A501A260}" name="Output Dimension" dataDxfId="5">
       <calculatedColumnFormula>Table134[[#This Row],[M]]*Table134[[#This Row],[K]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{17395CC5-C66A-45BB-AF44-85F63C798FE8}" name="MAC Count (Active PEs)"/>
-    <tableColumn id="6" xr3:uid="{F344959C-0D04-4AF5-B2C4-FF7C3F674B16}" name="Latency (Theory)" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{F344959C-0D04-4AF5-B2C4-FF7C3F674B16}" name="Latency (Theory)" dataDxfId="4">
       <calculatedColumnFormula>Table134[[#This Row],[M]]+Table134[[#This Row],[N]]+Table134[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{7EEC49AA-4FC8-4A99-9663-A8EEB2AAD5F8}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{B71F4CFD-5FC5-4951-83D9-6674EB7FB889}" name="Difference from 3N-2+1" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{B71F4CFD-5FC5-4951-83D9-6674EB7FB889}" name="Difference from 3N-2+1" dataDxfId="3">
       <calculatedColumnFormula>23-Table134[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -616,7 +1702,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA1FDD35-9C8D-43D3-A42C-5D9448260A9A}" name="Table1" displayName="Table1" ref="A2:H10" totalsRowShown="0">
   <autoFilter ref="A2:H10" xr:uid="{BA1FDD35-9C8D-43D3-A42C-5D9448260A9A}"/>
   <tableColumns count="8">
@@ -624,14 +1710,14 @@
     <tableColumn id="2" xr3:uid="{66D560B9-2DA7-4986-B3DE-CDA502776AC3}" name="M"/>
     <tableColumn id="3" xr3:uid="{5141C682-632F-43C2-8191-BB3609DB4DA8}" name="N"/>
     <tableColumn id="4" xr3:uid="{A9660E6C-180E-485D-A7EB-A8BFCE0C1D97}" name="K"/>
-    <tableColumn id="5" xr3:uid="{34B7FFF0-3EF6-4BA4-A5AB-1660E75007C8}" name="Output Dimension (MAC Count)" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{34B7FFF0-3EF6-4BA4-A5AB-1660E75007C8}" name="Output Dimension (MAC Count)" dataDxfId="2">
       <calculatedColumnFormula>4*8</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{3CE6D932-CF3F-4780-8775-A3AC543F142B}" name="Latency">
       <calculatedColumnFormula>Table1[[#This Row],[M]]+Table1[[#This Row],[N]]+Table1[[#This Row],[K]]-2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{3D0DE0B8-37A2-4603-B02E-4FE79DF8244C}" name="Latency (Real)"/>
-    <tableColumn id="8" xr3:uid="{78C59BA1-4582-42E9-8A9A-782701EF4A8A}" name="Difference from 3N-2+1" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{78C59BA1-4582-42E9-8A9A-782701EF4A8A}" name="Difference from 3N-2+1" dataDxfId="1">
       <calculatedColumnFormula>23-Table1[[#This Row],[Latency (Real)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -902,10 +1988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EAF263-E46A-4974-93A7-B91CE9F0B8F1}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,16 +2004,18 @@
     <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B1" s="7"/>
       <c r="D1" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -935,8 +2023,12 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -956,16 +2048,22 @@
         <v>3</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -973,7 +2071,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -994,8 +2092,14 @@
         <f>23-I3</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1024,8 +2128,14 @@
         <f t="shared" ref="J4:J11" si="0">23-I4</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1054,8 +2164,14 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>20</v>
+      </c>
+      <c r="M5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1084,8 +2200,14 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>30</v>
+      </c>
+      <c r="M6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1114,8 +2236,14 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>40</v>
+      </c>
+      <c r="M7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1144,8 +2272,14 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>50</v>
+      </c>
+      <c r="M8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1174,8 +2308,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>60</v>
+      </c>
+      <c r="M9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1204,8 +2344,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>70</v>
+      </c>
+      <c r="M10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1213,7 +2359,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" s="3">
         <v>8</v>
@@ -1234,17 +2380,58 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L11">
+        <v>75</v>
+      </c>
+      <c r="M11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>80</v>
+      </c>
+      <c r="M12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>85</v>
+      </c>
+      <c r="M13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>90</v>
+      </c>
+      <c r="M14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>95</v>
+      </c>
+      <c r="M15">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:J1"/>
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1268,12 +2455,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="G1" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -1283,16 +2470,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -1300,17 +2487,17 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C10" si="0">3*8-1</f>
         <v>23</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -1318,17 +2505,17 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -1336,17 +2523,17 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H5">
         <v>8</v>
@@ -1354,17 +2541,17 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6">
         <v>11</v>
@@ -1372,17 +2559,17 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H7">
         <v>14</v>
@@ -1390,17 +2577,17 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H8">
         <v>17</v>
@@ -1408,17 +2595,17 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H9">
         <v>20</v>
@@ -1426,17 +2613,17 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10">
         <v>23</v>
@@ -1460,7 +2647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB20B19-942C-4446-8EF3-236D33D3564C}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="134" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="134" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>

</xml_diff>